<commit_message>
final draft ready for final QA
</commit_message>
<xml_diff>
--- a/docs/extension-multipleAnd.xlsx
+++ b/docs/extension-multipleAnd.xlsx
@@ -137,7 +137,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>Whether multiple values are allowed for each time the parameter exists. Values are separated by commas, and the parameter matches if any of the values match.</t>
+    <t>Whether multiple parameters are allowed - e.g. more than one parameter with the same name. The search matches if all the parameters match.</t>
   </si>
   <si>
     <t>*</t>
@@ -406,7 +406,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="144.51953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="128.9765625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>